<commit_message>
'feats' - alex - Dum 17 Apr 2022 10:26:44 EEST - mac.local
</commit_message>
<xml_diff>
--- a/foaie_parcurs_B-151-VGT_martie_2022_Alex_Bora.xlsx
+++ b/foaie_parcurs_B-151-VGT_martie_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="37">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,45 +70,42 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Baia-Mare</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
+  </si>
+  <si>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Zalau</t>
+  </si>
+  <si>
     <t>Cluj-Cluj</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
-  </si>
-  <si>
     <t>Cluj-Turda</t>
   </si>
   <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Apahida</t>
-  </si>
-  <si>
     <t>Km parcursi:</t>
   </si>
   <si>
@@ -127,7 +124,7 @@
     <t>Total km Personal Ratio		 0,0%</t>
   </si>
   <si>
-    <t>Semnătură utilizator:			  Data predarii: 10.04.2022</t>
+    <t>Semnătură utilizator:			  Data predarii: 17.04.2022</t>
   </si>
   <si>
     <t>……………………………………………………</t>
@@ -641,7 +638,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>0</v>
+        <v>52375</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -663,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="4">
-        <v>47</v>
+        <v>356</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -677,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4">
-        <v>421</v>
+        <v>152</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -691,10 +688,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="4">
-        <v>257</v>
+        <v>356</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>18</v>
@@ -705,10 +702,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="4">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>18</v>
@@ -719,10 +716,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="4">
-        <v>152</v>
+        <v>85</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>18</v>
@@ -736,10 +733,10 @@
         <v>30</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1">
@@ -747,10 +744,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="4">
-        <v>101</v>
+        <v>257</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>18</v>
@@ -764,10 +761,10 @@
         <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -775,13 +772,13 @@
         <v>9</v>
       </c>
       <c r="B31" s="4">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="20" customHeight="1">
@@ -789,13 +786,13 @@
         <v>10</v>
       </c>
       <c r="B33" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20" customHeight="1">
@@ -803,10 +800,10 @@
         <v>11</v>
       </c>
       <c r="B35" s="4">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>18</v>
@@ -817,13 +814,13 @@
         <v>12</v>
       </c>
       <c r="B37" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="20" customHeight="1">
@@ -831,10 +828,10 @@
         <v>13</v>
       </c>
       <c r="B39" s="4">
-        <v>156</v>
+        <v>421</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>18</v>
@@ -845,10 +842,10 @@
         <v>14</v>
       </c>
       <c r="B41" s="4">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>18</v>
@@ -859,10 +856,10 @@
         <v>15</v>
       </c>
       <c r="B43" s="4">
-        <v>421</v>
+        <v>257</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>18</v>
@@ -873,10 +870,10 @@
         <v>16</v>
       </c>
       <c r="B45" s="4">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>18</v>
@@ -890,7 +887,7 @@
         <v>356</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>18</v>
@@ -901,13 +898,13 @@
         <v>18</v>
       </c>
       <c r="B49" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="20" customHeight="1">
@@ -918,10 +915,10 @@
         <v>30</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="20" customHeight="1">
@@ -929,7 +926,7 @@
         <v>20</v>
       </c>
       <c r="B53" s="4">
-        <v>356</v>
+        <v>121</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>28</v>
@@ -943,10 +940,10 @@
         <v>21</v>
       </c>
       <c r="B55" s="4">
-        <v>156</v>
+        <v>356</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>18</v>
@@ -957,10 +954,10 @@
         <v>22</v>
       </c>
       <c r="B57" s="4">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>18</v>
@@ -971,7 +968,7 @@
         <v>23</v>
       </c>
       <c r="B59" s="4">
-        <v>101</v>
+        <v>421</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>25</v>
@@ -985,10 +982,10 @@
         <v>24</v>
       </c>
       <c r="B61" s="4">
-        <v>421</v>
+        <v>101</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>18</v>
@@ -999,13 +996,13 @@
         <v>25</v>
       </c>
       <c r="B63" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="20" customHeight="1">
@@ -1013,13 +1010,13 @@
         <v>26</v>
       </c>
       <c r="B65" s="4">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="20" customHeight="1">
@@ -1027,10 +1024,10 @@
         <v>27</v>
       </c>
       <c r="B67" s="4">
-        <v>92</v>
+        <v>356</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>18</v>
@@ -1044,10 +1041,10 @@
         <v>30</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="20" customHeight="1">
@@ -1055,10 +1052,10 @@
         <v>29</v>
       </c>
       <c r="B71" s="4">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>18</v>
@@ -1069,10 +1066,10 @@
         <v>30</v>
       </c>
       <c r="B73" s="4">
-        <v>421</v>
+        <v>356</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>18</v>
@@ -1083,10 +1080,10 @@
         <v>31</v>
       </c>
       <c r="B75" s="4">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>18</v>
@@ -1094,48 +1091,48 @@
     </row>
     <row r="76" spans="1:4" ht="20" customHeight="1">
       <c r="A76" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="5">
-        <v>4803</v>
+        <v>5415</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="20" customHeight="1">
       <c r="A77" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B77" s="5">
-        <v>4803</v>
+        <v>57790</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="20" customHeight="1">
       <c r="A81" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="20" customHeight="1">
       <c r="A82" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="20" customHeight="1">
       <c r="A83" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="20" customHeight="1">
       <c r="A85" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="20" customHeight="1">
       <c r="A87" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="20" customHeight="1">
       <c r="A89" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>